<commit_message>
Fixed import function for new equipment categories
</commit_message>
<xml_diff>
--- a/Data/EQ Category Export.xlsx
+++ b/Data/EQ Category Export.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python\GCIEQ\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08AE1DF7-AB2F-4080-8926-16A440A92FD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A89D3B4-06CD-49F1-842B-13A6930378A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5490" yWindow="1110" windowWidth="21600" windowHeight="14370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29970" yWindow="1110" windowWidth="21600" windowHeight="14370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EQ Categories" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>eq_category_no</t>
   </si>
@@ -182,6 +182,12 @@
   </si>
   <si>
     <t>Test</t>
+  </si>
+  <si>
+    <t>YYYY</t>
+  </si>
+  <si>
+    <t>Tewst</t>
   </si>
 </sst>
 </file>
@@ -550,19 +556,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -570,7 +576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -578,7 +584,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -586,7 +592,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -594,7 +600,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -602,7 +608,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -610,7 +616,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -618,7 +624,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -626,7 +632,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -634,7 +640,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -642,7 +648,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -650,7 +656,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -658,7 +664,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -666,7 +672,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -674,7 +680,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -682,7 +688,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -690,7 +696,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -698,7 +704,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -706,7 +712,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -714,7 +720,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -722,7 +728,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -730,7 +736,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -738,7 +744,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -746,7 +752,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -754,7 +760,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -762,7 +768,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>50</v>
       </c>
@@ -776,6 +782,14 @@
       </c>
       <c r="B27" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>